<commit_message>
Test dir - openpyxl for Excel
</commit_message>
<xml_diff>
--- a/tutorial/test.xlsx
+++ b/tutorial/test.xlsx
@@ -13,32 +13,10 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Hello, World!</t>
-  </si>
-  <si>
-    <t>It's me!!!!</t>
-  </si>
-  <si>
-    <t>Bold</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,9 +44,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,31 +340,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>